<commit_message>
Remove obsolete files and update configurations for vmapi-vm. Deleted 50unattended-upgrades and readme.md files to streamline the setup process. Added new versions of inventory.xlsx and ip assignments.xlsx to reflect current network configurations and IP assignments.
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Projects\infrastructure-vm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Foundry\infrastructure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEE51DE7-BE04-4018-A25A-BAF1543BFF03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF132C9-C0A0-433E-95E6-39175F762FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{26DA0691-9C6D-4E5B-B4A5-C9DB0BC119FF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{26DA0691-9C6D-4E5B-B4A5-C9DB0BC119FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Servers" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="119">
   <si>
     <t>Memmory</t>
   </si>
@@ -163,18 +163,9 @@
     <t>CRS317-1-g16+</t>
   </si>
   <si>
-    <t>1B</t>
-  </si>
-  <si>
-    <t>1A</t>
-  </si>
-  <si>
     <t>Netgear</t>
   </si>
   <si>
-    <t>RB5009</t>
-  </si>
-  <si>
     <t>Desc</t>
   </si>
   <si>
@@ -241,9 +232,6 @@
     <t>usb mouse</t>
   </si>
   <si>
-    <t>hh00a5r8nxq/434</t>
-  </si>
-  <si>
     <t>hg309hzfknc/r2</t>
   </si>
   <si>
@@ -404,6 +392,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>CCR2116</t>
   </si>
 </sst>
 </file>
@@ -452,7 +443,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -465,6 +456,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -803,7 +797,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4AB5FB9-1A48-459E-8DA3-DCA682EBF1A9}">
   <dimension ref="A1:M47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
@@ -817,19 +811,19 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="F1" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -928,43 +922,43 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="J6" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>91</v>
-      </c>
       <c r="L6" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -972,13 +966,13 @@
         <v>17</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>19</v>
@@ -1013,13 +1007,13 @@
         <v>18</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>19</v>
@@ -1051,7 +1045,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1059,54 +1053,54 @@
         <v>0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>11</v>
@@ -1132,7 +1126,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>11</v>
@@ -1143,7 +1137,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>13</v>
@@ -1152,12 +1146,12 @@
         <v>13</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="J16" s="4" t="s">
         <v>13</v>
@@ -1166,12 +1160,12 @@
         <v>13</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="J17" s="4" t="s">
         <v>13</v>
@@ -1180,12 +1174,12 @@
         <v>13</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G18" s="4" t="s">
         <v>13</v>
@@ -1205,7 +1199,7 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>14</v>
@@ -1222,7 +1216,7 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>13</v>
@@ -1245,13 +1239,13 @@
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E22" s="4" t="s">
         <v>20</v>
@@ -1286,13 +1280,13 @@
         <v>25</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>24</v>
@@ -1324,16 +1318,16 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>21</v>
@@ -1365,56 +1359,56 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>116</v>
-      </c>
       <c r="C28" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1422,13 +1416,13 @@
         <v>2</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>16</v>
@@ -1481,7 +1475,7 @@
         <v>15</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I32" s="4" t="s">
         <v>15</v>
@@ -1504,7 +1498,7 @@
         <v>29</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F34" s="4" t="s">
         <v>31</v>
@@ -1513,19 +1507,19 @@
         <v>33</v>
       </c>
       <c r="H34" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="I34" s="4" t="s">
+      <c r="K34" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="L34" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="M34" s="4" t="s">
         <v>30</v>
@@ -1536,13 +1530,13 @@
         <v>22</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E36" s="4" t="s">
         <v>23</v>
@@ -1574,7 +1568,7 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -1589,7 +1583,7 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E47" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1601,10 +1595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D8E155-3FF9-4CD0-9FFA-93DF8D592C06}">
-  <dimension ref="A2:H8"/>
+  <dimension ref="A2:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F25:F26"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,7 +1611,7 @@
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>34</v>
@@ -1640,7 +1634,7 @@
         <v>45292</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>39</v>
@@ -1652,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1660,19 +1654,19 @@
         <v>45292</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2">
         <v>1</v>
       </c>
       <c r="F5" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1680,7 +1674,7 @@
         <v>45658</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>39</v>
@@ -1695,50 +1689,27 @@
         <v>4</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
-        <v>45658</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>49</v>
+      <c r="A7" s="6">
+        <v>45972</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>118</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>45658</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>41</v>
+      <c r="F7" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1750,8 +1721,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75BC87E7-57A1-4C6B-9845-7119B5CDBFD5}">
   <dimension ref="A2:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,10 +1746,10 @@
         <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
         <v>38</v>
@@ -1789,10 +1760,10 @@
         <v>45292</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1803,7 +1774,7 @@
         <v>45292</v>
       </c>
       <c r="D5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E5">
         <v>10</v>
@@ -1814,7 +1785,7 @@
         <v>45292</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E6">
         <v>10</v>
@@ -1825,7 +1796,7 @@
         <v>45292</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E7">
         <v>3</v>
@@ -1836,13 +1807,13 @@
         <v>45658</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E8">
         <v>4</v>
@@ -1853,13 +1824,13 @@
         <v>45658</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E9">
         <v>20</v>
@@ -1870,19 +1841,19 @@
         <v>45658</v>
       </c>
       <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
         <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1890,10 +1861,10 @@
         <v>45658</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E11">
         <v>1</v>

</xml_diff>